<commit_message>
added firm csvs and ppt
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdougherty1\Desktop\Nuveen summer 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obsid\Dropbox\Emeritus\capstone-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B56AC00-7689-4B29-B386-99DAE1BB20E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5D85E3-1A42-445B-96B9-F6A734D375F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2775" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary(MonthlyMetrics)" sheetId="6" r:id="rId1"/>
@@ -32,6 +32,65 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Daniel Wright</author>
+  </authors>
+  <commentList>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{17C1A68C-B684-44DD-8686-9FAF48182D4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Daniel Wright:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+assets under management equity
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{80F95080-ABA3-4113-A2C4-C69D62D3F664}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Daniel Wright:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+assets under managements municipal bonds</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
@@ -234,13 +293,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -410,6 +482,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,11 +750,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:AN41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B38"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,5 +1088,6 @@
     <mergeCell ref="C33:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>